<commit_message>
chore[doc]: update project timeline
</commit_message>
<xml_diff>
--- a/docs/ProjectTimeline/prjTimeline_QuanNguyen.xlsx
+++ b/docs/ProjectTimeline/prjTimeline_QuanNguyen.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HPHNNGCQUAN\LaneDetection_Thesis2022-23\docs\ProjectTimeline\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDFA3DEB-606E-4636-8A0F-B020CF394B5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A08EFAF-F915-4E3D-9503-6B2FAC2CD9A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Solution Offer</t>
   </si>
@@ -70,13 +70,28 @@
   </si>
   <si>
     <t>Device</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ha Phan Ngoc Quan </t>
+  </si>
+  <si>
+    <t>Truong Thanh Nguyen</t>
+  </si>
+  <si>
+    <t>To do</t>
+  </si>
+  <si>
+    <t>Doing</t>
+  </si>
+  <si>
+    <t>Done</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -84,16 +99,73 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -101,12 +173,93 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="1" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -387,93 +540,385 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A15"/>
+  <dimension ref="A1:R18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" zoomScale="76" zoomScaleNormal="76" workbookViewId="0">
+      <selection activeCell="U13" sqref="U13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.6640625" customWidth="1"/>
+    <col min="1" max="1" width="35.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A1" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="12">
+        <v>19145008</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A2" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="13">
+        <v>19145158</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" ht="20" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="7"/>
+      <c r="B3" s="4">
+        <v>44856</v>
+      </c>
+      <c r="C3" s="4">
+        <v>44887</v>
+      </c>
+      <c r="D3" s="4">
+        <v>44917</v>
+      </c>
+      <c r="E3" s="4">
+        <v>44584</v>
+      </c>
+      <c r="F3" s="4">
+        <v>44615</v>
+      </c>
+      <c r="G3" s="4">
+        <v>44643</v>
+      </c>
+      <c r="H3" s="4">
+        <v>44674</v>
+      </c>
+      <c r="I3" s="4">
+        <v>44704</v>
+      </c>
+      <c r="J3" s="4">
+        <v>44735</v>
+      </c>
+      <c r="K3" s="4">
+        <v>44765</v>
+      </c>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+      <c r="P3" s="2"/>
+    </row>
+    <row r="4" spans="1:18" ht="20" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="B4" s="14"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="9"/>
+      <c r="K4" s="9"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
+      <c r="Q4" s="15"/>
+      <c r="R4" s="18" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" ht="20" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="B5" s="19"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1"/>
+      <c r="P5" s="1"/>
+      <c r="Q5" s="16"/>
+      <c r="R5" s="18" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" ht="20" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="6" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="B6" s="19"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="9"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+      <c r="P6" s="1"/>
+      <c r="Q6" s="17"/>
+      <c r="R6" s="18" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" ht="20" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="B7" s="19"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="9"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="1"/>
+    </row>
+    <row r="8" spans="1:18" ht="20" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="6" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="B8" s="19"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="9"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+      <c r="P8" s="1"/>
+    </row>
+    <row r="9" spans="1:18" ht="20" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="9"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+      <c r="P9" s="1"/>
+    </row>
+    <row r="10" spans="1:18" ht="20" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="6" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="B10" s="9"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9"/>
+      <c r="K10" s="9"/>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1"/>
+      <c r="P10" s="1"/>
+    </row>
+    <row r="11" spans="1:18" ht="20" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="9"/>
+      <c r="K11" s="9"/>
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
+      <c r="P11" s="1"/>
+    </row>
+    <row r="12" spans="1:18" ht="20" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="6" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="9"/>
+      <c r="K12" s="9"/>
+      <c r="L12" s="1"/>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
+      <c r="O12" s="1"/>
+      <c r="P12" s="1"/>
+    </row>
+    <row r="13" spans="1:18" ht="20" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+      <c r="B13" s="9"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="9"/>
+      <c r="K13" s="9"/>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+      <c r="P13" s="1"/>
+    </row>
+    <row r="14" spans="1:18" ht="20" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="6" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+      <c r="B14" s="9"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="9"/>
+      <c r="J14" s="9"/>
+      <c r="K14" s="9"/>
+      <c r="L14" s="1"/>
+      <c r="M14" s="1"/>
+      <c r="N14" s="1"/>
+      <c r="O14" s="1"/>
+      <c r="P14" s="1"/>
+    </row>
+    <row r="15" spans="1:18" ht="20" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+      <c r="B15" s="9"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="9"/>
+      <c r="K15" s="9"/>
+      <c r="L15" s="1"/>
+      <c r="M15" s="1"/>
+      <c r="N15" s="1"/>
+      <c r="O15" s="1"/>
+      <c r="P15" s="1"/>
+    </row>
+    <row r="16" spans="1:18" ht="20" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="6" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+      <c r="B16" s="10"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="8"/>
+      <c r="J16" s="8"/>
+      <c r="K16" s="9"/>
+      <c r="L16" s="1"/>
+      <c r="M16" s="1"/>
+      <c r="N16" s="1"/>
+      <c r="O16" s="1"/>
+      <c r="P16" s="1"/>
+    </row>
+    <row r="17" spans="1:16" ht="20" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+      <c r="B17" s="8"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="8"/>
+      <c r="I17" s="8"/>
+      <c r="J17" s="8"/>
+      <c r="K17" s="11"/>
+      <c r="L17" s="1"/>
+      <c r="M17" s="1"/>
+      <c r="N17" s="1"/>
+      <c r="O17" s="1"/>
+      <c r="P17" s="1"/>
+    </row>
+    <row r="18" spans="1:16" ht="20" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="6" t="s">
         <v>12</v>
       </c>
+      <c r="B18" s="10"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="11"/>
+      <c r="J18" s="8"/>
+      <c r="K18" s="11"/>
+      <c r="L18" s="1"/>
+      <c r="M18" s="1"/>
+      <c r="N18" s="1"/>
+      <c r="O18" s="1"/>
+      <c r="P18" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
chore[docs]: update  docs according to timeline
</commit_message>
<xml_diff>
--- a/docs/ProjectTimeline/prjTimeline_QuanNguyen.xlsx
+++ b/docs/ProjectTimeline/prjTimeline_QuanNguyen.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gitHub\thesis\LaneDetection_Thesis2022-23\docs\ProjectTimeline\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HPHNNGCQUAN\LaneDetection_Thesis2022-23\docs\ProjectTimeline\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C091CF30-0AA5-4DF5-B58B-B254B5166F27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3BA9C9C-5B79-4C7B-9267-A356E0D50343}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="2280" yWindow="2280" windowWidth="14400" windowHeight="7810" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -95,7 +95,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -103,14 +103,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF00B050"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -225,7 +225,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -252,6 +252,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -534,20 +536,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" zoomScale="81" zoomScaleNormal="81" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="35.109375" customWidth="1"/>
+    <col min="1" max="1" width="35.08203125" customWidth="1"/>
+    <col min="2" max="2" width="9.4140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="9">
+      <c r="B1" s="18">
         <v>19145008</v>
       </c>
       <c r="J1" s="17"/>
@@ -562,7 +565,7 @@
       <c r="A2" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="10">
+      <c r="B2" s="19">
         <v>19145158</v>
       </c>
       <c r="J2" s="17"/>
@@ -573,7 +576,7 @@
       <c r="O2" s="17"/>
       <c r="P2" s="17"/>
     </row>
-    <row r="3" spans="1:16" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" ht="20" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5"/>
       <c r="B3" s="2">
         <v>44856</v>
@@ -609,7 +612,7 @@
       <c r="O3" s="17"/>
       <c r="P3" s="17"/>
     </row>
-    <row r="4" spans="1:16" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" ht="20" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>0</v>
       </c>
@@ -631,11 +634,11 @@
       <c r="O4" s="17"/>
       <c r="P4" s="17"/>
     </row>
-    <row r="5" spans="1:16" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" ht="20" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="16"/>
+      <c r="B5" s="11"/>
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
       <c r="E5" s="7"/>
@@ -653,7 +656,7 @@
       <c r="O5" s="17"/>
       <c r="P5" s="17"/>
     </row>
-    <row r="6" spans="1:16" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" ht="20" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>1</v>
       </c>
@@ -673,7 +676,7 @@
       <c r="O6" s="17"/>
       <c r="P6" s="17"/>
     </row>
-    <row r="7" spans="1:16" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" ht="20" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
@@ -693,7 +696,7 @@
       <c r="O7" s="17"/>
       <c r="P7" s="17"/>
     </row>
-    <row r="8" spans="1:16" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" ht="20" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>2</v>
       </c>
@@ -713,7 +716,7 @@
       <c r="O8" s="17"/>
       <c r="P8" s="17"/>
     </row>
-    <row r="9" spans="1:16" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" ht="20" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -733,7 +736,7 @@
       <c r="O9" s="17"/>
       <c r="P9" s="17"/>
     </row>
-    <row r="10" spans="1:16" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" ht="20" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>3</v>
       </c>
@@ -752,7 +755,7 @@
       <c r="O10" s="17"/>
       <c r="P10" s="17"/>
     </row>
-    <row r="11" spans="1:16" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16" ht="20" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>5</v>
       </c>
@@ -772,7 +775,7 @@
       <c r="O11" s="17"/>
       <c r="P11" s="17"/>
     </row>
-    <row r="12" spans="1:16" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16" ht="20" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>18</v>
       </c>
@@ -792,7 +795,7 @@
       <c r="O12" s="17"/>
       <c r="P12" s="17"/>
     </row>
-    <row r="13" spans="1:16" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16" ht="20" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>4</v>
       </c>
@@ -812,7 +815,7 @@
       <c r="O13" s="17"/>
       <c r="P13" s="17"/>
     </row>
-    <row r="14" spans="1:16" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16" ht="20" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>8</v>
       </c>
@@ -831,7 +834,7 @@
       <c r="O14" s="17"/>
       <c r="P14" s="17"/>
     </row>
-    <row r="15" spans="1:16" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16" ht="20" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>19</v>
       </c>
@@ -850,7 +853,7 @@
       <c r="O15" s="17"/>
       <c r="P15" s="17"/>
     </row>
-    <row r="16" spans="1:16" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16" ht="20" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>12</v>
       </c>
@@ -870,7 +873,7 @@
       <c r="O16" s="17"/>
       <c r="P16" s="17"/>
     </row>
-    <row r="17" spans="1:16" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:16" ht="20" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>10</v>
       </c>
@@ -890,7 +893,7 @@
       <c r="O17" s="17"/>
       <c r="P17" s="17"/>
     </row>
-    <row r="18" spans="1:16" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:16" ht="20" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
         <v>11</v>
       </c>

</xml_diff>

<commit_message>
chore[docs]: update timeline - Dec 2022
</commit_message>
<xml_diff>
--- a/docs/ProjectTimeline/prjTimeline_QuanNguyen.xlsx
+++ b/docs/ProjectTimeline/prjTimeline_QuanNguyen.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gitHub\thesis\LaneDetection_Thesis2022-23\docs\ProjectTimeline\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gitHub\LaneDetection-OpenCV\docs\ProjectTimeline\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CE23B11-6810-4032-B819-359A2F4C7BD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFB6A781-10DA-4F65-A4AA-18D2E4C25534}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -255,9 +255,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="16" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -267,21 +267,18 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
@@ -564,50 +561,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P18"/>
+  <dimension ref="A1:L18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O7" sqref="O7"/>
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.109375" customWidth="1"/>
-    <col min="2" max="9" width="10.77734375" customWidth="1"/>
-    <col min="11" max="11" width="10.77734375" customWidth="1"/>
+    <col min="1" max="1" width="35.140625" customWidth="1"/>
+    <col min="2" max="9" width="10.7109375" customWidth="1"/>
+    <col min="11" max="11" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="18">
+      <c r="B1" s="15">
         <v>19145008</v>
       </c>
-      <c r="J1" s="17"/>
-      <c r="K1" s="17"/>
-      <c r="L1" s="17"/>
-      <c r="M1" s="17"/>
-      <c r="N1" s="17"/>
-      <c r="O1" s="17"/>
-      <c r="P1" s="17"/>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A2" s="10" t="s">
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="19">
+      <c r="B2" s="16">
         <v>19145158</v>
       </c>
-      <c r="J2" s="17"/>
-      <c r="K2" s="17"/>
-      <c r="L2" s="17"/>
-      <c r="M2" s="17"/>
-      <c r="N2" s="17"/>
-      <c r="O2" s="17"/>
-      <c r="P2" s="17"/>
-    </row>
-    <row r="3" spans="1:16" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:12" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5"/>
       <c r="B3" s="2" t="s">
         <v>27</v>
@@ -633,21 +616,16 @@
       <c r="I3" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="J3" s="17"/>
-      <c r="K3" s="12"/>
-      <c r="L3" s="15" t="s">
+      <c r="K3" s="11"/>
+      <c r="L3" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="M3" s="17"/>
-      <c r="N3" s="17"/>
-      <c r="O3" s="17"/>
-      <c r="P3" s="17"/>
-    </row>
-    <row r="4" spans="1:16" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:12" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="11"/>
+      <c r="B4" s="10"/>
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
@@ -655,21 +633,16 @@
       <c r="G4" s="7"/>
       <c r="H4" s="7"/>
       <c r="I4" s="7"/>
-      <c r="J4" s="17"/>
-      <c r="K4" s="13"/>
-      <c r="L4" s="15" t="s">
+      <c r="K4" s="12"/>
+      <c r="L4" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="M4" s="17"/>
-      <c r="N4" s="17"/>
-      <c r="O4" s="17"/>
-      <c r="P4" s="17"/>
-    </row>
-    <row r="5" spans="1:16" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:12" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="11"/>
+      <c r="B5" s="10"/>
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
       <c r="E5" s="7"/>
@@ -677,21 +650,16 @@
       <c r="G5" s="7"/>
       <c r="H5" s="7"/>
       <c r="I5" s="7"/>
-      <c r="J5" s="17"/>
-      <c r="K5" s="14"/>
-      <c r="L5" s="15" t="s">
+      <c r="K5" s="13"/>
+      <c r="L5" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="M5" s="17"/>
-      <c r="N5" s="17"/>
-      <c r="O5" s="17"/>
-      <c r="P5" s="17"/>
-    </row>
-    <row r="6" spans="1:16" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:12" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="11"/>
+      <c r="B6" s="10"/>
       <c r="C6" s="7"/>
       <c r="D6" s="7"/>
       <c r="E6" s="7"/>
@@ -699,19 +667,12 @@
       <c r="G6" s="7"/>
       <c r="H6" s="7"/>
       <c r="I6" s="7"/>
-      <c r="J6" s="17"/>
-      <c r="K6" s="17"/>
-      <c r="L6" s="17"/>
-      <c r="M6" s="17"/>
-      <c r="N6" s="17"/>
-      <c r="O6" s="17"/>
-      <c r="P6" s="17"/>
-    </row>
-    <row r="7" spans="1:16" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:12" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="16"/>
+      <c r="B7" s="13"/>
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
       <c r="E7" s="7"/>
@@ -719,19 +680,12 @@
       <c r="G7" s="7"/>
       <c r="H7" s="7"/>
       <c r="I7" s="7"/>
-      <c r="J7" s="17"/>
-      <c r="K7" s="17"/>
-      <c r="L7" s="17"/>
-      <c r="M7" s="17"/>
-      <c r="N7" s="17"/>
-      <c r="O7" s="17"/>
-      <c r="P7" s="17"/>
-    </row>
-    <row r="8" spans="1:16" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:12" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="16"/>
+      <c r="B8" s="13"/>
       <c r="C8" s="7"/>
       <c r="D8" s="7"/>
       <c r="E8" s="7"/>
@@ -739,54 +693,33 @@
       <c r="G8" s="7"/>
       <c r="H8" s="7"/>
       <c r="I8" s="7"/>
-      <c r="J8" s="17"/>
-      <c r="K8" s="17"/>
-      <c r="L8" s="17"/>
-      <c r="M8" s="17"/>
-      <c r="N8" s="17"/>
-      <c r="O8" s="17"/>
-      <c r="P8" s="17"/>
-    </row>
-    <row r="9" spans="1:16" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:12" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B9" s="13"/>
-      <c r="C9" s="6"/>
+      <c r="C9" s="12"/>
       <c r="D9" s="7"/>
       <c r="E9" s="7"/>
       <c r="F9" s="7"/>
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
       <c r="I9" s="7"/>
-      <c r="J9" s="17"/>
-      <c r="K9" s="17"/>
-      <c r="L9" s="17"/>
-      <c r="M9" s="17"/>
-      <c r="N9" s="17"/>
-      <c r="O9" s="17"/>
-      <c r="P9" s="17"/>
-    </row>
-    <row r="10" spans="1:16" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:12" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B10" s="7"/>
-      <c r="C10" s="6"/>
+      <c r="C10" s="12"/>
       <c r="D10" s="6"/>
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
       <c r="H10" s="7"/>
       <c r="I10" s="7"/>
-      <c r="J10" s="17"/>
-      <c r="K10" s="17"/>
-      <c r="L10" s="17"/>
-      <c r="M10" s="17"/>
-      <c r="N10" s="17"/>
-      <c r="O10" s="17"/>
-      <c r="P10" s="17"/>
-    </row>
-    <row r="11" spans="1:16" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:12" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>5</v>
       </c>
@@ -794,19 +727,12 @@
       <c r="C11" s="7"/>
       <c r="D11" s="6"/>
       <c r="E11" s="6"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
       <c r="H11" s="7"/>
       <c r="I11" s="7"/>
-      <c r="J11" s="17"/>
-      <c r="K11" s="17"/>
-      <c r="L11" s="17"/>
-      <c r="M11" s="17"/>
-      <c r="N11" s="17"/>
-      <c r="O11" s="17"/>
-      <c r="P11" s="17"/>
-    </row>
-    <row r="12" spans="1:16" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:12" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>18</v>
       </c>
@@ -818,35 +744,21 @@
       <c r="G12" s="6"/>
       <c r="H12" s="7"/>
       <c r="I12" s="7"/>
-      <c r="J12" s="17"/>
-      <c r="K12" s="17"/>
-      <c r="L12" s="17"/>
-      <c r="M12" s="17"/>
-      <c r="N12" s="17"/>
-      <c r="O12" s="17"/>
-      <c r="P12" s="17"/>
-    </row>
-    <row r="13" spans="1:16" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:12" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B13" s="7"/>
       <c r="C13" s="7"/>
       <c r="D13" s="7"/>
-      <c r="E13" s="8"/>
+      <c r="E13" s="7"/>
       <c r="F13" s="6"/>
       <c r="G13" s="6"/>
       <c r="H13" s="6"/>
       <c r="I13" s="7"/>
-      <c r="J13" s="17"/>
-      <c r="K13" s="17"/>
-      <c r="L13" s="17"/>
-      <c r="M13" s="17"/>
-      <c r="N13" s="17"/>
-      <c r="O13" s="17"/>
-      <c r="P13" s="17"/>
-    </row>
-    <row r="14" spans="1:16" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:12" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>8</v>
       </c>
@@ -857,15 +769,8 @@
       <c r="G14" s="6"/>
       <c r="H14" s="6"/>
       <c r="I14" s="7"/>
-      <c r="J14" s="17"/>
-      <c r="K14" s="17"/>
-      <c r="L14" s="17"/>
-      <c r="M14" s="17"/>
-      <c r="N14" s="17"/>
-      <c r="O14" s="17"/>
-      <c r="P14" s="17"/>
-    </row>
-    <row r="15" spans="1:16" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:12" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>26</v>
       </c>
@@ -876,73 +781,45 @@
       <c r="G15" s="6"/>
       <c r="H15" s="6"/>
       <c r="I15" s="7"/>
-      <c r="J15" s="17"/>
-      <c r="K15" s="17"/>
-      <c r="L15" s="17"/>
-      <c r="M15" s="17"/>
-      <c r="N15" s="17"/>
-      <c r="O15" s="17"/>
-      <c r="P15" s="17"/>
-    </row>
-    <row r="16" spans="1:16" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:12" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B16" s="8"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="8"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
       <c r="H16" s="6"/>
       <c r="I16" s="6"/>
-      <c r="J16" s="17"/>
-      <c r="K16" s="17"/>
-      <c r="L16" s="17"/>
-      <c r="M16" s="17"/>
-      <c r="N16" s="17"/>
-      <c r="O16" s="17"/>
-      <c r="P16" s="17"/>
-    </row>
-    <row r="17" spans="1:16" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:9" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B17" s="8"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
+      <c r="B17" s="7"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
       <c r="E17" s="6"/>
       <c r="F17" s="6"/>
       <c r="G17" s="6"/>
       <c r="H17" s="6"/>
       <c r="I17" s="6"/>
-      <c r="J17" s="17"/>
-      <c r="K17" s="17"/>
-      <c r="L17" s="17"/>
-      <c r="M17" s="17"/>
-      <c r="N17" s="17"/>
-      <c r="O17" s="17"/>
-      <c r="P17" s="17"/>
-    </row>
-    <row r="18" spans="1:16" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="1:9" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B18" s="8"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="8"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
       <c r="E18" s="7"/>
       <c r="F18" s="7"/>
-      <c r="G18" s="8"/>
+      <c r="G18" s="7"/>
       <c r="H18" s="6"/>
       <c r="I18" s="6"/>
-      <c r="J18" s="17"/>
-      <c r="K18" s="17"/>
-      <c r="L18" s="17"/>
-      <c r="M18" s="17"/>
-      <c r="N18" s="17"/>
-      <c r="O18" s="17"/>
-      <c r="P18" s="17"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>

</xml_diff>